<commit_message>
update results for task 2
</commit_message>
<xml_diff>
--- a/Promise/results_task2.xlsx
+++ b/Promise/results_task2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeit\Papiere\paper_req_classification\Datasets\Promise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74C84FC-277C-4C57-8409-430C0DAE4699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D58DD2-6E18-41F9-8973-A3D8AD397004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18120" yWindow="-5460" windowWidth="18240" windowHeight="28440" xr2:uid="{EAA1F360-018B-4C01-84E1-44DDC1521104}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="35">
   <si>
     <t>Model</t>
   </si>
@@ -196,12 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,8 +240,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33CEC9F1-A573-4EAA-A856-CCF7E23A9823}" name="Table1" displayName="Table1" ref="A2:U28" totalsRowShown="0">
-  <autoFilter ref="A2:U28" xr:uid="{46E8206C-B5D9-4847-B526-08C1427E16AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33CEC9F1-A573-4EAA-A856-CCF7E23A9823}" name="Table1" displayName="Table1" ref="A2:U30" totalsRowShown="0">
+  <autoFilter ref="A2:U30" xr:uid="{46E8206C-B5D9-4847-B526-08C1427E16AD}"/>
   <tableColumns count="21">
     <tableColumn id="21" xr3:uid="{72471577-5A2A-48E9-B471-BCD3377B4DD5}" name="Classifier" dataDxfId="0"/>
     <tableColumn id="1" xr3:uid="{2C10759C-0547-4F14-A016-676A07FCBEFE}" name="Fold"/>
@@ -565,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABB2A89-5550-4106-AF63-C8C8FC55BBED}">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,16 +1923,16 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <v>16</v>
@@ -1946,43 +1947,43 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J24">
-        <v>0.69</v>
+        <v>0.84</v>
       </c>
       <c r="K24">
-        <v>0.72</v>
+        <v>0.8</v>
       </c>
       <c r="L24">
+        <v>0.82</v>
+      </c>
+      <c r="M24">
+        <v>0.89</v>
+      </c>
+      <c r="N24">
+        <v>0.89</v>
+      </c>
+      <c r="O24">
+        <v>0.89</v>
+      </c>
+      <c r="P24">
+        <v>0.78</v>
+      </c>
+      <c r="Q24">
         <v>0.7</v>
       </c>
-      <c r="M24">
-        <v>0.8</v>
-      </c>
-      <c r="N24">
-        <v>0.83</v>
-      </c>
-      <c r="O24">
-        <v>0.81</v>
-      </c>
-      <c r="P24">
-        <v>0.79</v>
-      </c>
-      <c r="Q24">
-        <v>0.73</v>
-      </c>
       <c r="R24">
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
       <c r="S24">
         <v>0.91</v>
       </c>
       <c r="T24">
-        <v>0.56999999999999995</v>
+        <v>0.8</v>
       </c>
       <c r="U24">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -1993,7 +1994,7 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <v>16</v>
@@ -2014,51 +2015,51 @@
         <v>13</v>
       </c>
       <c r="J25">
-        <v>0.87</v>
+        <v>0.69</v>
       </c>
       <c r="K25">
+        <v>0.72</v>
+      </c>
+      <c r="L25">
         <v>0.7</v>
       </c>
-      <c r="L25">
-        <v>0.78</v>
-      </c>
       <c r="M25">
-        <v>0.89</v>
+        <v>0.8</v>
       </c>
       <c r="N25">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="O25">
-        <v>0.85</v>
+        <v>0.81</v>
       </c>
       <c r="P25">
-        <v>0.88</v>
+        <v>0.79</v>
       </c>
       <c r="Q25">
-        <v>0.79</v>
+        <v>0.73</v>
       </c>
       <c r="R25">
-        <v>0.83</v>
+        <v>0.76</v>
       </c>
       <c r="S25">
-        <v>0.89</v>
+        <v>0.91</v>
       </c>
       <c r="T25">
-        <v>0.78</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="U25">
-        <v>0.83</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>16</v>
@@ -2076,43 +2077,43 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J26">
-        <v>0.65</v>
+        <v>0.87</v>
       </c>
       <c r="K26">
+        <v>0.7</v>
+      </c>
+      <c r="L26">
         <v>0.78</v>
       </c>
-      <c r="L26">
-        <v>0.71</v>
-      </c>
       <c r="M26">
-        <v>0.77</v>
+        <v>0.89</v>
       </c>
       <c r="N26">
+        <v>0.82</v>
+      </c>
+      <c r="O26">
+        <v>0.85</v>
+      </c>
+      <c r="P26">
+        <v>0.88</v>
+      </c>
+      <c r="Q26">
+        <v>0.79</v>
+      </c>
+      <c r="R26">
+        <v>0.83</v>
+      </c>
+      <c r="S26">
         <v>0.89</v>
       </c>
-      <c r="O26">
+      <c r="T26">
+        <v>0.78</v>
+      </c>
+      <c r="U26">
         <v>0.83</v>
-      </c>
-      <c r="P26">
-        <v>0.67</v>
-      </c>
-      <c r="Q26">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="R26">
-        <v>0.61</v>
-      </c>
-      <c r="S26">
-        <v>0.86</v>
-      </c>
-      <c r="T26">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="U26">
-        <v>0.69</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -2126,10 +2127,10 @@
         <v>10</v>
       </c>
       <c r="D27">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E27">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F27">
         <v>0.75</v>
@@ -2138,46 +2139,46 @@
         <v>904727489</v>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
       </c>
       <c r="J27">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="K27">
-        <v>0.56999999999999995</v>
+        <v>0.78</v>
       </c>
       <c r="L27">
-        <v>0.64</v>
+        <v>0.71</v>
       </c>
       <c r="M27">
-        <v>0.69</v>
+        <v>0.77</v>
       </c>
       <c r="N27">
-        <v>0.76</v>
+        <v>0.89</v>
       </c>
       <c r="O27">
-        <v>0.72</v>
+        <v>0.83</v>
       </c>
       <c r="P27">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="Q27">
         <v>0.56000000000000005</v>
       </c>
       <c r="R27">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="S27">
-        <v>0.71</v>
+        <v>0.86</v>
       </c>
       <c r="T27">
-        <v>0.46</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="U27">
-        <v>0.56000000000000005</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -2203,7 +2204,7 @@
         <v>904727489</v>
       </c>
       <c r="H28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
@@ -2212,37 +2213,167 @@
         <v>0.75</v>
       </c>
       <c r="K28">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L28">
+        <v>0.64</v>
+      </c>
+      <c r="M28">
+        <v>0.69</v>
+      </c>
+      <c r="N28">
+        <v>0.76</v>
+      </c>
+      <c r="O28">
         <v>0.72</v>
       </c>
-      <c r="L28">
+      <c r="P28">
+        <v>0.71</v>
+      </c>
+      <c r="Q28">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R28">
+        <v>0.63</v>
+      </c>
+      <c r="S28">
+        <v>0.71</v>
+      </c>
+      <c r="T28">
+        <v>0.46</v>
+      </c>
+      <c r="U28">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
+      </c>
+      <c r="F29">
+        <v>0.75</v>
+      </c>
+      <c r="G29">
+        <v>904727489</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29">
+        <v>0.75</v>
+      </c>
+      <c r="K29">
+        <v>0.72</v>
+      </c>
+      <c r="L29">
         <v>0.73</v>
       </c>
-      <c r="M28">
+      <c r="M29">
         <v>0.73</v>
       </c>
-      <c r="N28">
+      <c r="N29">
         <v>0.88</v>
       </c>
-      <c r="O28">
+      <c r="O29">
         <v>0.8</v>
       </c>
-      <c r="P28">
+      <c r="P29">
         <v>0.72</v>
       </c>
-      <c r="Q28">
+      <c r="Q29">
         <v>0.57999999999999996</v>
       </c>
-      <c r="R28">
+      <c r="R29">
         <v>0.64</v>
       </c>
-      <c r="S28">
+      <c r="S29">
         <v>0.79</v>
       </c>
-      <c r="T28">
+      <c r="T29">
         <v>0.61</v>
       </c>
-      <c r="U28">
+      <c r="U29">
         <v>0.69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>0.75</v>
+      </c>
+      <c r="G30">
+        <v>904727489</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30">
+        <v>0.85</v>
+      </c>
+      <c r="K30">
+        <v>0.79</v>
+      </c>
+      <c r="L30">
+        <v>0.82</v>
+      </c>
+      <c r="M30">
+        <v>0.92</v>
+      </c>
+      <c r="N30">
+        <v>0.91</v>
+      </c>
+      <c r="O30">
+        <v>0.91</v>
+      </c>
+      <c r="P30">
+        <v>0.8</v>
+      </c>
+      <c r="Q30">
+        <v>0.77</v>
+      </c>
+      <c r="R30">
+        <v>0.79</v>
+      </c>
+      <c r="S30">
+        <v>0.86</v>
+      </c>
+      <c r="T30">
+        <v>0.81</v>
+      </c>
+      <c r="U30">
+        <v>0.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>